<commit_message>
add more Kd values measured by SPR and radioligand assay
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0848F0AF-B0B7-F644-B88E-3B78A336D4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D9D57C-7D41-494D-ABA4-C762973C60DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="740" windowWidth="22400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
   <si>
     <t>Reference</t>
   </si>
@@ -287,6 +287,15 @@
   </si>
   <si>
     <t>Tiedemann et al., 2002</t>
+  </si>
+  <si>
+    <t>Papadopoulos et al., 2012</t>
+  </si>
+  <si>
+    <t>Jin et al., 2007</t>
+  </si>
+  <si>
+    <t>Breier et al., 1995</t>
   </si>
 </sst>
 </file>
@@ -323,7 +332,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -542,24 +551,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -584,10 +580,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,7 +919,7 @@
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -966,19 +967,59 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
         <v>7.5</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>3</v>
       </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="24">
+        <v>9.33</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="19">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="22">
+        <v>114</v>
+      </c>
+      <c r="D8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
delete `Breier et al., 1995` data from VEGF:VEGFR1 Kd (radioligand)
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D9D57C-7D41-494D-ABA4-C762973C60DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE6B93D-FC19-E249-9E43-CB84EAD8E9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
   <si>
     <t>Reference</t>
   </si>
@@ -293,9 +293,6 @@
   </si>
   <si>
     <t>Jin et al., 2007</t>
-  </si>
-  <si>
-    <t>Breier et al., 1995</t>
   </si>
 </sst>
 </file>
@@ -555,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -583,12 +580,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,44 +973,32 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="24">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
         <v>9.33</v>
       </c>
       <c r="D6" s="6">
         <v>0.33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="8">
         <v>7</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="22">
-        <v>114</v>
-      </c>
-      <c r="D8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change the name `Tiedemann` -> `von Tiedemann`
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE6B93D-FC19-E249-9E43-CB84EAD8E9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F6A565-E151-BD4D-821B-8EF13D0F6229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -286,13 +286,13 @@
     <t>Teran et al., 2019 (monomer)</t>
   </si>
   <si>
-    <t>Tiedemann et al., 2002</t>
-  </si>
-  <si>
     <t>Papadopoulos et al., 2012</t>
   </si>
   <si>
     <t>Jin et al., 2007</t>
+  </si>
+  <si>
+    <t>von Tiedemann et al., 2002</t>
   </si>
 </sst>
 </file>
@@ -897,7 +897,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,7 +960,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>9</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Shobhan has not published yet -> change it into "Unpublished data"
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F6A565-E151-BD4D-821B-8EF13D0F6229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6665BE-0123-AB4F-944E-E74F549424C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -247,9 +247,6 @@
     <t>Mamer et al., 2020</t>
   </si>
   <si>
-    <t>Shobhan et al., 2023</t>
-  </si>
-  <si>
     <t>Huang et al., 1998 (VEGF-A165)</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>von Tiedemann et al., 2002</t>
+  </si>
+  <si>
+    <t>Unpublished data</t>
   </si>
 </sst>
 </file>
@@ -896,7 +896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -922,7 +922,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>8</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>9</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>8</v>
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="2" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>9</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1410,7 +1410,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add (Teran, 2019) data to VEGF:VEGFR1 and VEGF:VEGFR2 binding affinity
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6665BE-0123-AB4F-944E-E74F549424C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5EAD05-E257-A940-BD23-555EC9835D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="19400" yWindow="740" windowWidth="10000" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
   <si>
     <t>Reference</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>Unpublished data</t>
+  </si>
+  <si>
+    <t>Teran et al., 2019</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -548,11 +551,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -580,6 +622,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,18 +1034,32 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="20">
         <v>7</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="21">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="23">
+        <v>196</v>
+      </c>
+      <c r="D8" s="24">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1011,7 +1073,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1252,18 +1314,18 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="20">
         <f>AVERAGE(I12:I14)</f>
         <v>580</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="21">
         <f>STDEVA(I12:I14)/SQRT(3)</f>
         <v>156.31165450257808</v>
       </c>
@@ -1280,7 +1342,19 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="23">
+        <v>8600</v>
+      </c>
+      <c r="D11" s="24">
+        <v>500</v>
+      </c>
       <c r="G11" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
delete (Fuh, 2000) data from VEGF:NRP1 data
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5EAD05-E257-A940-BD23-555EC9835D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CD6714-8C5A-1C43-9FCB-6E7FEB2D7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19400" yWindow="740" windowWidth="10000" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="19400" yWindow="740" windowWidth="10000" windowHeight="16700" firstSheet="1" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -156,51 +156,8 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Yunjeong Lee</author>
-  </authors>
-  <commentList>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{E2BBAABC-FA0C-8F40-98A9-9861430A0343}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yunjeong Lee:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Error: ~35%</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
   <si>
     <t>Reference</t>
   </si>
@@ -272,9 +229,6 @@
   </si>
   <si>
     <t>Soker et al., 1998</t>
-  </si>
-  <si>
-    <t>Fuh et al., 2000</t>
   </si>
   <si>
     <t>Teran et al., 2019 (chimera)</t>
@@ -1008,7 +962,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>9</v>
@@ -1022,7 +976,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -1036,7 +990,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>8</v>
@@ -1050,7 +1004,7 @@
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>9</v>
@@ -1072,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1316,7 +1270,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>9</v>
@@ -1344,7 +1298,7 @@
     </row>
     <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>9</v>
@@ -1408,11 +1362,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1490,43 +1444,27 @@
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
-        <f>C6*0.35</f>
-        <v>39.549999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8">
         <v>25</v>
       </c>
-      <c r="D7" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="8">
-        <v>25</v>
-      </c>
-      <c r="D8" s="9">
+      <c r="D7" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add (Breier et al., 1995) to `VEGF:VEGFR1` sheet
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CD6714-8C5A-1C43-9FCB-6E7FEB2D7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5270D03-DF39-CF4F-9B2E-6FD695B18099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19400" yWindow="740" windowWidth="10000" windowHeight="16700" firstSheet="1" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
   <si>
     <t>Reference</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Teran et al., 2019</t>
+  </si>
+  <si>
+    <t>Breier et al., 1995</t>
   </si>
 </sst>
 </file>
@@ -548,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -579,9 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1002,19 +1003,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="23">
+      <c r="B8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="20">
         <v>196</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <v>4</v>
       </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="22">
+        <v>114</v>
+      </c>
+      <c r="D9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1297,16 +1310,16 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="23">
+      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8">
         <v>8600</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="9">
         <v>500</v>
       </c>
       <c r="G11" t="s">
@@ -1365,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
edit SE of [Papadopoulos et al., 2012)
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5270D03-DF39-CF4F-9B2E-6FD695B18099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE4CADC-7C3E-FA40-B6A4-239812B38F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,7 +986,7 @@
         <v>9.33</v>
       </c>
       <c r="D6" s="6">
-        <v>0.33</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add (Whitaker, 2001)'s SE
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE4CADC-7C3E-FA40-B6A4-239812B38F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15557336-29ED-0543-B788-53675B23ADCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -899,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,7 +1141,9 @@
       <c r="C4" s="1">
         <v>339</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7">
+        <v>120</v>
+      </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
@@ -1379,7 +1381,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1411,7 +1413,9 @@
       <c r="C2" s="2">
         <v>2.09</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6">
+        <v>0.82</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">

</xml_diff>

<commit_message>
Add (Ito & Claesson-Welsh, 1999) to VEGF:VEGFR1
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15557336-29ED-0543-B788-53675B23ADCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0042827-4998-8D4E-8942-106A597FAE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="33">
   <si>
     <t>Reference</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Breier et al., 1995</t>
+  </si>
+  <si>
+    <t>Ito &amp; Claesson-Welsh, 1999</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -582,6 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -897,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1017,17 +1021,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="20">
         <v>114</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="23">
+        <v>91.54</v>
+      </c>
+      <c r="D10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1039,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add (Gu et al., 2002) to VEGF:NRP1
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0042827-4998-8D4E-8942-106A597FAE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315EF51E-B1EE-0B42-9039-5A2B96B53C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
   <si>
     <t>Reference</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>Ito &amp; Claesson-Welsh, 1999</t>
+  </si>
+  <si>
+    <t>Gu et al., 2002</t>
   </si>
 </sst>
 </file>
@@ -903,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,7 +1059,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1483,18 +1486,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20">
         <v>25</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="21">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete (Waltenberger et al., 1994) using HUVEC from VEGF:VEGFR1 and VEGF:VEGFR2 sheets
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315EF51E-B1EE-0B42-9039-5A2B96B53C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80CDBA5-AF3F-F844-85A4-D53D912B5EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{F5752615-28CF-6E4E-A51C-5229D569314F}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{F5752615-28CF-6E4E-A51C-5229D569314F}">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
   <si>
     <t>Reference</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>Waltenberger et al., 1994 (PAE cell)</t>
-  </si>
-  <si>
-    <t>Waltenberger et al., 1994 (HUVEC)</t>
   </si>
   <si>
     <t>Cunningham et al., 1999 (pre-dimerized)</t>
@@ -557,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -588,8 +585,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,70 +939,72 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>9</v>
-      </c>
-      <c r="D3" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>9.33</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="20">
+        <v>7</v>
+      </c>
+      <c r="D6" s="21">
         <v>1</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="D5" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>9.33</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="20">
-        <v>7</v>
+        <v>196</v>
       </c>
       <c r="D7" s="21">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1015,38 +1012,24 @@
         <v>30</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="20">
-        <v>196</v>
-      </c>
-      <c r="D8" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="20">
-        <v>114</v>
-      </c>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="23">
+      <c r="C9" s="8">
         <v>91.54</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1059,7 +1042,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,12 +1188,14 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>770</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>37.1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="G6" t="s">
         <v>10</v>
       </c>
@@ -1232,10 +1217,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>37.1</v>
+        <v>51.7</v>
       </c>
       <c r="D7" s="7">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
@@ -1252,16 +1237,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>51.7</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D8" s="7">
-        <v>5.8</v>
+        <v>0.4</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -1277,17 +1262,19 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0.4</v>
+      <c r="A9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="20">
+        <f>AVERAGE(I12:I14)</f>
+        <v>580</v>
+      </c>
+      <c r="D9" s="21">
+        <f>STDEVA(I12:I14)/SQRT(3)</f>
+        <v>156.31165450257808</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -1302,20 +1289,18 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="20">
-        <f>AVERAGE(I12:I14)</f>
-        <v>580</v>
-      </c>
-      <c r="D10" s="21">
-        <f>STDEVA(I12:I14)/SQRT(3)</f>
-        <v>156.31165450257808</v>
+      <c r="B10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8">
+        <v>8600</v>
+      </c>
+      <c r="D10" s="9">
+        <v>500</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -1330,19 +1315,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8">
-        <v>8600</v>
-      </c>
-      <c r="D11" s="9">
-        <v>500</v>
-      </c>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G11" t="s">
         <v>3</v>
       </c>
@@ -1399,7 +1372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1438,7 +1411,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1450,7 +1423,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1462,7 +1435,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1474,7 +1447,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -1488,7 +1461,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>9</v>
@@ -1501,13 +1474,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="23" t="s">
+      <c r="A8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="8">
         <v>0.93</v>
       </c>
       <c r="D8" s="9">

</xml_diff>

<commit_message>
change reference label from `Waltenberger et al., 1994 (PAE cell)` to `Waltenberger et al., 1994`
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80CDBA5-AF3F-F844-85A4-D53D912B5EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3FDB25-8E10-244E-A0FE-017D1A22536D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t>Huang et al., 1998 (VEGF-A164)</t>
   </si>
   <si>
-    <t>Waltenberger et al., 1994 (PAE cell)</t>
-  </si>
-  <si>
     <t>Cunningham et al., 1999 (pre-dimerized)</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>Gu et al., 2002</t>
+  </si>
+  <si>
+    <t>Waltenberger et al., 1994</t>
   </si>
 </sst>
 </file>
@@ -902,7 +902,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,7 +927,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>9</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>8</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>9</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>8</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>8</v>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>9</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>9</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>9</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
delete `Soker et al., 1996 (HUVEC)` from `VEGFA165_NRP1` sheet
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3FDB25-8E10-244E-A0FE-017D1A22536D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB47834D-F6AE-CB4E-AEC2-9CC2CBEA690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
   <si>
     <t>Reference</t>
   </si>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>Cunningham et al., 1999 (monomer)</t>
-  </si>
-  <si>
-    <t>Soker et al., 1996 (HUVEC)</t>
   </si>
   <si>
     <t>Soker et al., 1996 (breast cancer cell)</t>
@@ -901,7 +898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -927,7 +924,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -953,7 +950,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>9</v>
@@ -967,7 +964,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -981,7 +978,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>8</v>
@@ -995,7 +992,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>9</v>
@@ -1009,7 +1006,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>8</v>
@@ -1021,7 +1018,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>8</v>
@@ -1161,7 +1158,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1263,7 +1260,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>9</v>
@@ -1291,7 +1288,7 @@
     </row>
     <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>9</v>
@@ -1370,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1417,7 +1414,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>0.2</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -1429,7 +1426,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.32</v>
       </c>
       <c r="D4" s="7"/>
     </row>
@@ -1438,52 +1435,40 @@
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>25</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="20">
+        <v>25</v>
+      </c>
+      <c r="D6" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.32</v>
-      </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="20">
-        <v>25</v>
-      </c>
-      <c r="D7" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="C7" s="8">
         <v>0.93</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D7" s="9">
         <v>0.71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change the reference label from `Soker et al., 1996 (HUVEC)` to `Soker et al., 1996`
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB47834D-F6AE-CB4E-AEC2-9CC2CBEA690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB796A5-DE79-7046-BF73-04D9F3AA6FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -216,9 +216,6 @@
     <t>Cunningham et al., 1999 (monomer)</t>
   </si>
   <si>
-    <t>Soker et al., 1996 (breast cancer cell)</t>
-  </si>
-  <si>
     <t>Soker et al., 1998</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>Waltenberger et al., 1994</t>
+  </si>
+  <si>
+    <t>Soker et al., 1996</t>
   </si>
 </sst>
 </file>
@@ -924,7 +924,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>9</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>8</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>9</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>8</v>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>8</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>9</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>9</v>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>9</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add Shobhan's data to VEGF:NRP1 sheet
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB796A5-DE79-7046-BF73-04D9F3AA6FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC069D71-B3F3-AC4C-B3A8-A0FD5FA30075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
   <si>
     <t>Reference</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Soker et al., 1996</t>
+  </si>
+  <si>
+    <t>Shobhan, 2023</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -582,6 +585,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1367,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1378,7 +1383,7 @@
     <col min="1" max="1" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1392,7 +1397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>13</v>
       </c>
@@ -1405,8 +1410,14 @@
       <c r="D2" s="6">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>5.29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>31</v>
       </c>
@@ -1417,8 +1428,11 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>7.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>19</v>
       </c>
@@ -1430,7 +1444,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>20</v>
       </c>
@@ -1444,7 +1458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>21</v>
       </c>
@@ -1458,18 +1472,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="20">
         <v>0.93</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="21">
         <v>0.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8">
+        <f>AVERAGE(G2:G3)</f>
+        <v>6.3599999999999994</v>
+      </c>
+      <c r="D8" s="9">
+        <f>STDEVA(G2:G3)/SQRT(2)</f>
+        <v>1.0700000000000032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add `Terman et al., 1992` to VEGF165:VEGFR2 sheet
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC069D71-B3F3-AC4C-B3A8-A0FD5FA30075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A05304-86C4-A440-8D0B-FC577D95D2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="34">
   <si>
     <t>Reference</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>Shobhan, 2023</t>
+  </si>
+  <si>
+    <t>Terman et al., 1992</t>
   </si>
 </sst>
 </file>
@@ -554,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -585,8 +588,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1043,7 +1044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1136,18 +1137,16 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
-        <v>339</v>
-      </c>
-      <c r="D4" s="7">
-        <v>120</v>
-      </c>
+      <c r="C4" s="2">
+        <v>75</v>
+      </c>
+      <c r="D4" s="6"/>
       <c r="G4" t="s">
         <v>6</v>
       </c>
@@ -1163,15 +1162,17 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>760</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>339</v>
+      </c>
+      <c r="D5" s="7">
+        <v>120</v>
+      </c>
       <c r="G5" t="s">
         <v>6</v>
       </c>
@@ -1187,17 +1188,15 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>37.1</v>
-      </c>
-      <c r="D6" s="7">
-        <v>4.9000000000000004</v>
-      </c>
+        <v>760</v>
+      </c>
+      <c r="D6" s="7"/>
       <c r="G6" t="s">
         <v>10</v>
       </c>
@@ -1213,16 +1212,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>51.7</v>
+        <v>37.1</v>
       </c>
       <c r="D7" s="7">
-        <v>5.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
@@ -1239,16 +1238,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>9.8000000000000007</v>
+        <v>51.7</v>
       </c>
       <c r="D8" s="7">
-        <v>0.4</v>
+        <v>5.8</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -1264,46 +1263,46 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>37.1</v>
+      </c>
+      <c r="J9">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="20">
+      <c r="B10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="20">
         <f>AVERAGE(I12:I14)</f>
         <v>580</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D10" s="21">
         <f>STDEVA(I12:I14)/SQRT(3)</f>
         <v>156.31165450257808</v>
       </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9">
-        <v>37.1</v>
-      </c>
-      <c r="J9">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8">
-        <v>8600</v>
-      </c>
-      <c r="D10" s="9">
-        <v>500</v>
-      </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
@@ -1317,7 +1316,19 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8">
+        <v>8600</v>
+      </c>
+      <c r="D11" s="9">
+        <v>500</v>
+      </c>
       <c r="G11" t="s">
         <v>3</v>
       </c>
@@ -1374,7 +1385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1487,10 +1498,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="8">

</xml_diff>

<commit_message>
change value for `Ito & Claesson-Welsh, 1999` from 91.54 pM to 54 pM in VEGF:VEGFR1 sheet
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A05304-86C4-A440-8D0B-FC577D95D2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC059099-5FFB-AE44-AB9B-7FF25177803F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1030,7 +1030,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="8">
-        <v>91.54</v>
+        <v>54</v>
       </c>
       <c r="D9" s="9"/>
     </row>
@@ -1044,7 +1044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add binding affinity data measured in HUVEC in (Waltenberger et al., 1994) and (Soker et al., 1996)
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC059099-5FFB-AE44-AB9B-7FF25177803F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B06C32-4A84-7849-880F-EA1C57318CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{F5752615-28CF-6E4E-A51C-5229D569314F}">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{F5752615-28CF-6E4E-A51C-5229D569314F}">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
   <si>
     <t>Reference</t>
   </si>
@@ -249,16 +249,25 @@
     <t>Gu et al., 2002</t>
   </si>
   <si>
-    <t>Waltenberger et al., 1994</t>
-  </si>
-  <si>
-    <t>Soker et al., 1996</t>
-  </si>
-  <si>
     <t>Shobhan, 2023</t>
   </si>
   <si>
     <t>Terman et al., 1992</t>
+  </si>
+  <si>
+    <t>Waltenberger et al., 1994 (PAE cells)</t>
+  </si>
+  <si>
+    <t>Waltenberger et al., 1994 (HUVEC)</t>
+  </si>
+  <si>
+    <t>Waltenberger et al., 1994 (PAE cell)</t>
+  </si>
+  <si>
+    <t>Soker et al., 1996 (MDA-MB-231)</t>
+  </si>
+  <si>
+    <t>Soker et al., 1996 (HUVEC)</t>
   </si>
 </sst>
 </file>
@@ -902,15 +911,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -930,7 +939,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -941,98 +950,110 @@
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.3</v>
-      </c>
+      <c r="A3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
         <v>7.5</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D5" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
         <v>9.33</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D6" s="6">
         <v>0.71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="20">
-        <v>7</v>
-      </c>
-      <c r="D6" s="21">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="20">
-        <v>196</v>
+        <v>7</v>
       </c>
       <c r="D7" s="21">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="20">
+        <v>196</v>
+      </c>
+      <c r="D8" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="20">
+      <c r="B9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="20">
         <v>114</v>
       </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8">
         <v>54</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1045,12 +1066,12 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1138,7 +1159,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1188,7 +1209,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1212,17 +1233,15 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>37.1</v>
-      </c>
-      <c r="D7" s="7">
-        <v>4.9000000000000004</v>
-      </c>
+        <v>770</v>
+      </c>
+      <c r="D7" s="7"/>
       <c r="G7" t="s">
         <v>1</v>
       </c>
@@ -1238,16 +1257,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>51.7</v>
+        <v>37.1</v>
       </c>
       <c r="D8" s="7">
-        <v>5.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -1264,16 +1283,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>9.8000000000000007</v>
+        <v>51.7</v>
       </c>
       <c r="D9" s="7">
-        <v>0.4</v>
+        <v>5.8</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -1289,46 +1308,46 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>51.7</v>
+      </c>
+      <c r="J10">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="20">
+      <c r="B11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="20">
         <f>AVERAGE(I12:I14)</f>
         <v>580</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D11" s="21">
         <f>STDEVA(I12:I14)/SQRT(3)</f>
         <v>156.31165450257808</v>
       </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10">
-        <v>51.7</v>
-      </c>
-      <c r="J10">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8">
-        <v>8600</v>
-      </c>
-      <c r="D11" s="9">
-        <v>500</v>
-      </c>
       <c r="G11" t="s">
         <v>3</v>
       </c>
@@ -1342,7 +1361,19 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8">
+        <v>8600</v>
+      </c>
+      <c r="D12" s="9">
+        <v>500</v>
+      </c>
       <c r="G12" t="s">
         <v>12</v>
       </c>
@@ -1383,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1422,93 +1453,105 @@
         <v>0.82</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2">
         <v>5.29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D3" s="7"/>
+      <c r="A3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="6"/>
       <c r="G3">
         <v>7.43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>0.32</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
         <v>25</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D6" s="7">
         <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="20">
-        <v>25</v>
-      </c>
-      <c r="D6" s="21">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20">
+        <v>25</v>
+      </c>
+      <c r="D7" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="20">
+      <c r="B8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="20">
         <v>0.93</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D8" s="21">
         <v>0.71</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8">
         <f>AVERAGE(G2:G3)</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D9" s="9">
         <f>STDEVA(G2:G3)/SQRT(2)</f>
         <v>1.0700000000000032</v>
       </c>

</xml_diff>

<commit_message>
delete (Teran et al., 2019) data from VEGF:VEGFR1 and VEGF:VEGFR2
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B06C32-4A84-7849-880F-EA1C57318CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAA3B02-9D4F-3B43-B732-7655FD466AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="36">
   <si>
     <t>Reference</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>Unpublished data</t>
-  </si>
-  <si>
-    <t>Teran et al., 2019</t>
   </si>
   <si>
     <t>Breier et al., 1995</t>
@@ -911,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -939,7 +936,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -951,7 +948,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>8</v>
@@ -1022,38 +1019,24 @@
         <v>26</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="20">
-        <v>196</v>
-      </c>
-      <c r="D8" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="20">
-        <v>114</v>
-      </c>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8">
         <v>54</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1065,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1159,7 +1142,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1209,7 +1192,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1233,7 +1216,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1308,16 +1291,16 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="B10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="20">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="21">
         <v>0.4</v>
       </c>
       <c r="G10" t="s">
@@ -1333,18 +1316,18 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="20">
+      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8">
         <f>AVERAGE(I12:I14)</f>
         <v>580</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="9">
         <f>STDEVA(I12:I14)/SQRT(3)</f>
         <v>156.31165450257808</v>
       </c>
@@ -1361,19 +1344,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="8">
-        <v>8600</v>
-      </c>
-      <c r="D12" s="9">
-        <v>500</v>
-      </c>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G12" t="s">
         <v>12</v>
       </c>
@@ -1416,7 +1387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1453,7 +1424,7 @@
         <v>0.82</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2">
         <v>5.29</v>
@@ -1461,7 +1432,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1476,7 +1447,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1528,7 +1499,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
edit typo in VEGF:VEGFR1 (`PAE cells` -> `PAE cell`) for consistency
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAA3B02-9D4F-3B43-B732-7655FD466AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC36091-1377-244B-8B16-A172C0B405EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
   <si>
     <t>Reference</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>Terman et al., 1992</t>
-  </si>
-  <si>
-    <t>Waltenberger et al., 1994 (PAE cells)</t>
   </si>
   <si>
     <t>Waltenberger et al., 1994 (HUVEC)</t>
@@ -910,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,7 +933,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -948,7 +945,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>8</v>
@@ -1048,7 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1192,7 +1189,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1216,7 +1213,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1432,7 +1429,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1447,7 +1444,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
delete (Teran et al., 2019) data from VEGF:NRP1
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC36091-1377-244B-8B16-A172C0B405EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5C4C12-C4DB-2148-B7A8-12EBDAD0B2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
   <si>
     <t>Reference</t>
   </si>
@@ -217,12 +217,6 @@
   </si>
   <si>
     <t>Soker et al., 1998</t>
-  </si>
-  <si>
-    <t>Teran et al., 2019 (chimera)</t>
-  </si>
-  <si>
-    <t>Teran et al., 2019 (monomer)</t>
   </si>
   <si>
     <t>Papadopoulos et al., 2012</t>
@@ -907,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -933,7 +927,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -945,7 +939,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>8</v>
@@ -971,7 +965,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>9</v>
@@ -985,7 +979,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -999,7 +993,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>8</v>
@@ -1013,7 +1007,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>8</v>
@@ -1025,7 +1019,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>8</v>
@@ -1139,7 +1133,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1189,7 +1183,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1213,7 +1207,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1315,7 +1309,7 @@
     </row>
     <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
@@ -1382,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1421,7 +1415,7 @@
         <v>0.82</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G2">
         <v>5.29</v>
@@ -1429,7 +1423,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1444,7 +1438,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1467,59 +1461,31 @@
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="20">
-        <v>25</v>
-      </c>
-      <c r="D7" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="20">
+      <c r="A6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="20">
         <v>0.93</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D6" s="21">
         <v>0.71</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="8">
+    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8">
         <f>AVERAGE(G2:G3)</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D7" s="9">
         <f>STDEVA(G2:G3)/SQRT(2)</f>
         <v>1.0700000000000032</v>
       </c>

</xml_diff>

<commit_message>
add (Peach et al., 2018) data to VEGF:NRP1
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5C4C12-C4DB-2148-B7A8-12EBDAD0B2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE2A211-9402-A543-81B3-D60A17485A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="35">
   <si>
     <t>Reference</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>Soker et al., 1996 (HUVEC)</t>
+  </si>
+  <si>
+    <t>Peach et al., 2018</t>
+  </si>
+  <si>
+    <t>NanoBret</t>
   </si>
 </sst>
 </file>
@@ -554,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -585,6 +591,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1474,18 +1482,32 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="23">
+        <v>4.95</v>
+      </c>
+      <c r="D7" s="21">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8">
         <f>AVERAGE(G2:G3)</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D8" s="9">
         <f>STDEVA(G2:G3)/SQRT(2)</f>
         <v>1.0700000000000032</v>
       </c>

</xml_diff>

<commit_message>
delete (Peach et al., 2018) data to VEGF:NRP1
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE2A211-9402-A543-81B3-D60A17485A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18052280-76D1-1F40-8DE0-BE975F4FFC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
   <si>
     <t>Reference</t>
   </si>
@@ -256,12 +256,6 @@
   </si>
   <si>
     <t>Soker et al., 1996 (HUVEC)</t>
-  </si>
-  <si>
-    <t>Peach et al., 2018</t>
-  </si>
-  <si>
-    <t>NanoBret</t>
   </si>
 </sst>
 </file>
@@ -560,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -591,8 +585,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1482,32 +1474,18 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="23">
-        <v>4.95</v>
-      </c>
-      <c r="D7" s="21">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8">
         <f>AVERAGE(G2:G3)</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D7" s="9">
         <f>STDEVA(G2:G3)/SQRT(2)</f>
         <v>1.0700000000000032</v>
       </c>

</xml_diff>

<commit_message>
edit standard error of VEGF:VEGFR1 binding affinity in (Papadopoulos et al., 2012)
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18052280-76D1-1F40-8DE0-BE975F4FFC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5090319D-E9F3-474C-AF4F-B8079D849947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -901,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,7 +988,7 @@
         <v>9.33</v>
       </c>
       <c r="D6" s="6">
-        <v>0.71</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1378,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
`Cunningham et al., 1999 (pre-dimerized)` -> `Cunningham et al., 1999 (predimer)`
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5090319D-E9F3-474C-AF4F-B8079D849947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92476EEA-4997-1643-8744-426514264730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -210,9 +210,6 @@
     <t>Huang et al., 1998 (VEGF-A164)</t>
   </si>
   <si>
-    <t>Cunningham et al., 1999 (pre-dimerized)</t>
-  </si>
-  <si>
     <t>Cunningham et al., 1999 (monomer)</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>Soker et al., 1996 (HUVEC)</t>
+  </si>
+  <si>
+    <t>Cunningham et al., 1999 (predimer)</t>
   </si>
 </sst>
 </file>
@@ -901,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -927,7 +927,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>8</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>9</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>8</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>8</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>8</v>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
@@ -1415,7 +1415,7 @@
         <v>0.82</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2">
         <v>5.29</v>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>8</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
update SE [Tidemann, 2002] by dividing the original value by sqrt(10)
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92476EEA-4997-1643-8744-426514264730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F28B95-DAC7-2E4E-B23E-8AB35CA4070B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -901,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -974,7 +974,8 @@
         <v>7.5</v>
       </c>
       <c r="D5" s="7">
-        <v>3</v>
+        <f>3/SQRT(10)</f>
+        <v>0.94868329805051377</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1039,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
change `Unpublished data` to `In-house data`
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F28B95-DAC7-2E4E-B23E-8AB35CA4070B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3659F370-930C-284D-9B68-EC191F995FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -225,9 +225,6 @@
     <t>von Tiedemann et al., 2002</t>
   </si>
   <si>
-    <t>Unpublished data</t>
-  </si>
-  <si>
     <t>Breier et al., 1995</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>Cunningham et al., 1999 (predimer)</t>
+  </si>
+  <si>
+    <t>In-house data</t>
   </si>
 </sst>
 </file>
@@ -901,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -927,7 +927,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>8</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>8</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>8</v>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
@@ -1379,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
@@ -1416,7 +1416,7 @@
         <v>0.82</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2">
         <v>5.29</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>8</v>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add Rouet et al.'s data
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3659F370-930C-284D-9B68-EC191F995FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA710B7-10DD-704E-A982-4E0E042B6469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="35">
   <si>
     <t>Reference</t>
   </si>
@@ -256,13 +256,19 @@
   </si>
   <si>
     <t>In-house data</t>
+  </si>
+  <si>
+    <t>Rouet et al., 2005</t>
+  </si>
+  <si>
+    <t>ELISA plate+Saturation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,6 +289,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -554,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -567,13 +580,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -585,6 +596,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -912,10 +928,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -926,10 +942,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2">
@@ -938,10 +954,10 @@
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2">
@@ -950,10 +966,10 @@
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1">
@@ -964,10 +980,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1">
@@ -979,7 +995,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -993,42 +1009,56 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="20">
+      <c r="B7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="18">
         <v>7</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="20">
+      <c r="B8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="18">
         <v>114</v>
       </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="18">
         <v>54</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="21">
+        <v>59.4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>19.600000000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1041,7 +1071,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1054,13 +1084,13 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -1077,7 +1107,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1105,7 +1135,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1133,7 +1163,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1157,7 +1187,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1183,7 +1213,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1207,7 +1237,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1231,7 +1261,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1257,7 +1287,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1283,16 +1313,16 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="20">
+      <c r="B10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="18">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="19">
         <v>0.4</v>
       </c>
       <c r="G10" t="s">
@@ -1308,18 +1338,18 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="B11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="18">
         <f>AVERAGE(I12:I14)</f>
         <v>580</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="19">
         <f>STDEVA(I12:I14)/SQRT(3)</f>
         <v>156.31165450257808</v>
       </c>
@@ -1336,7 +1366,19 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="21">
+        <v>292.5</v>
+      </c>
+      <c r="D12" s="22">
+        <v>163.80000000000001</v>
+      </c>
       <c r="G12" t="s">
         <v>12</v>
       </c>
@@ -1377,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1392,18 +1434,18 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1423,7 +1465,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1438,7 +1480,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1450,7 +1492,7 @@
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1462,33 +1504,47 @@
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="20">
+      <c r="B6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="18">
         <v>0.93</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="19">
         <v>0.71</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="18">
         <f>AVERAGE(G2:G3)</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="19">
         <f>STDEVA(G2:G3)/SQRT(2)</f>
         <v>1.0700000000000032</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="21">
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.1351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change names of Shobhan's data from `In-house data` to `In-house data, 2023`
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA710B7-10DD-704E-A982-4E0E042B6469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96599A9-6CEA-CC4D-A4EB-F6BEC7E0E216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -255,13 +255,13 @@
     <t>Cunningham et al., 1999 (predimer)</t>
   </si>
   <si>
-    <t>In-house data</t>
-  </si>
-  <si>
     <t>Rouet et al., 2005</t>
   </si>
   <si>
     <t>ELISA plate+Saturation</t>
+  </si>
+  <si>
+    <t>In-house data, 2023</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -596,9 +596,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -917,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1048,10 +1047,10 @@
     </row>
     <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="C10" s="21">
         <v>59.4</v>
@@ -1071,7 +1070,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,7 +1339,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>9</v>
@@ -1368,15 +1367,15 @@
     </row>
     <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="C12" s="21">
         <v>292.5</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="8">
         <v>163.80000000000001</v>
       </c>
       <c r="G12" t="s">
@@ -1421,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1519,7 +1518,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>9</v>
@@ -1534,11 +1533,11 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>34</v>
       </c>
       <c r="C8" s="21">
         <v>0.24640000000000001</v>

</xml_diff>

<commit_message>
change `von Tiedemann et al., 2002` -> `von Tiedemann & Bilitewski, 2002`
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96599A9-6CEA-CC4D-A4EB-F6BEC7E0E216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286629CB-6095-2C44-8CFA-AD697C82FF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>Jin et al., 2007</t>
   </si>
   <si>
-    <t>von Tiedemann et al., 2002</t>
-  </si>
-  <si>
     <t>Breier et al., 1995</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>In-house data, 2023</t>
+  </si>
+  <si>
+    <t>von Tiedemann &amp; Bilitewski, 2002</t>
   </si>
 </sst>
 </file>
@@ -917,7 +917,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,7 +942,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>8</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>8</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>9</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>8</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>8</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>32</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>33</v>
       </c>
       <c r="C10" s="21">
         <v>59.4</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>9</v>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>33</v>
       </c>
       <c r="C12" s="21">
         <v>292.5</v>
@@ -1457,7 +1457,7 @@
         <v>0.82</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>5.29</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>8</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>9</v>
@@ -1534,10 +1534,10 @@
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>33</v>
       </c>
       <c r="C8" s="21">
         <v>0.24640000000000001</v>

</xml_diff>

<commit_message>
add [Lu, 2023] and [Herve, 2008] data to VEGF:VEGFR2 and VEGF:NRP1 sheets
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286629CB-6095-2C44-8CFA-AD697C82FF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A656E12D-2822-5742-B6CD-1AFCD4BF5A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
   <si>
     <t>Reference</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>von Tiedemann &amp; Bilitewski, 2002</t>
+  </si>
+  <si>
+    <t>Lu et al., 2023</t>
+  </si>
+  <si>
+    <t>Herve et al., 2008</t>
   </si>
 </sst>
 </file>
@@ -305,7 +311,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -487,87 +493,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -588,18 +518,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -930,7 +854,7 @@
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -944,7 +868,7 @@
       <c r="A2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2">
@@ -953,22 +877,22 @@
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6"/>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1">
@@ -982,7 +906,7 @@
       <c r="A5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1">
@@ -994,65 +918,65 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
         <v>9.33</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>0.96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="18">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
         <v>7</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="18">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
         <v>114</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="18">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
         <v>54</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="15">
         <v>59.4</v>
       </c>
       <c r="D10" s="8">
@@ -1070,7 +994,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,17 +1058,17 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
         <f>AVERAGE(I4:I5)</f>
         <v>235</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <f>STDEVA(I4:I5)/SQRT(2)</f>
         <v>95</v>
       </c>
@@ -1162,16 +1086,16 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
         <v>75</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="7"/>
       <c r="G4" t="s">
         <v>6</v>
       </c>
@@ -1312,16 +1236,16 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="18">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="7">
         <v>0.4</v>
       </c>
       <c r="G10" t="s">
@@ -1338,17 +1262,17 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="18">
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
         <f>AVERAGE(I12:I14)</f>
         <v>580</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="7">
         <f>STDEVA(I12:I14)/SQRT(3)</f>
         <v>156.31165450257808</v>
       </c>
@@ -1365,17 +1289,17 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="1">
         <v>292.5</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>163.80000000000001</v>
       </c>
       <c r="G12" t="s">
@@ -1388,7 +1312,19 @@
         <v>700</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="15">
+        <v>115.406329531968</v>
+      </c>
+      <c r="D13" s="8">
+        <v>73.439181551013107</v>
+      </c>
       <c r="G13" t="s">
         <v>12</v>
       </c>
@@ -1418,10 +1354,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1464,16 +1400,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
         <v>0.2</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="7"/>
       <c r="G3">
         <v>7.43</v>
       </c>
@@ -1503,47 +1439,75 @@
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="18">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.93</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="7">
         <v>0.71</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="18">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
         <f>AVERAGE(G2:G3)</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="7">
         <f>STDEVA(G2:G3)/SQRT(2)</f>
         <v>1.0700000000000032</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="1">
         <v>0.24640000000000001</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>0.1351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.6940999814534656</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.8337311851513098</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0.1450937334938032</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5.8905524473255033E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete 700 pM from Shobhan's data in the VEGF:VEGFR2 Kd dataset
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A656E12D-2822-5742-B6CD-1AFCD4BF5A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E58ADBB-56B5-E14F-9D33-62319759EEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="37">
   <si>
     <t>Reference</t>
   </si>
@@ -497,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -521,9 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,10 +989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,12 +1267,12 @@
         <v>9</v>
       </c>
       <c r="C11" s="1">
-        <f>AVERAGE(I12:I14)</f>
-        <v>580</v>
+        <f>AVERAGE(I12:I13)</f>
+        <v>520</v>
       </c>
       <c r="D11" s="7">
-        <f>STDEVA(I12:I14)/SQRT(3)</f>
-        <v>156.31165450257808</v>
+        <f>STDEVA(I12:I13)/SQRT(2)</f>
+        <v>250</v>
       </c>
       <c r="G11" t="s">
         <v>3</v>
@@ -1309,7 +1307,7 @@
         <v>9</v>
       </c>
       <c r="I12">
-        <v>700</v>
+        <v>770</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1332,17 +1330,6 @@
         <v>9</v>
       </c>
       <c r="I13">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14">
         <v>270</v>
       </c>
     </row>
@@ -1356,7 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1469,7 +1456,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -1486,7 +1473,7 @@
       <c r="A9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1">
@@ -1500,7 +1487,7 @@
       <c r="A10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="15">

</xml_diff>

<commit_message>
add (Papadopoulos et al., 2012) data to VEGF:VEGFR2
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E58ADBB-56B5-E14F-9D33-62319759EEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D969B95-784E-CE46-86F3-2C63D8F65184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
   <si>
     <t>Reference</t>
   </si>
@@ -311,7 +311,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -493,11 +493,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -522,6 +561,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -989,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1310,17 +1355,17 @@
         <v>770</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="15">
+      <c r="B13" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="19">
         <v>115.406329531968</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="20">
         <v>73.439181551013107</v>
       </c>
       <c r="G13" t="s">
@@ -1331,6 +1376,20 @@
       </c>
       <c r="I13">
         <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="22">
+        <v>88.8</v>
+      </c>
+      <c r="D14" s="23">
+        <v>6.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Whitaker and von Tidemann's missing data
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D969B95-784E-CE46-86F3-2C63D8F65184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1826268F-F0B9-4741-A471-1CBBA39F5DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>Reference</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Shobhan2023</t>
   </si>
   <si>
-    <t>Whitaker et al., 2001</t>
-  </si>
-  <si>
     <t>Mamer et al., 2020</t>
   </si>
   <si>
@@ -261,13 +258,25 @@
     <t>In-house data, 2023</t>
   </si>
   <si>
-    <t>von Tiedemann &amp; Bilitewski, 2002</t>
-  </si>
-  <si>
     <t>Lu et al., 2023</t>
   </si>
   <si>
     <t>Herve et al., 2008</t>
+  </si>
+  <si>
+    <t>von Tiedemann &amp; Bilitewski, 2002 (SPR)</t>
+  </si>
+  <si>
+    <t>von Tiedemann &amp; Bilitewski, 2002 (Radioligand)</t>
+  </si>
+  <si>
+    <t>Soker et al., 1996</t>
+  </si>
+  <si>
+    <t>Whitaker et al., 2001 (COS-1 cell)</t>
+  </si>
+  <si>
+    <t>Whitaker et al., 2001 (Balb/c cell)</t>
   </si>
 </sst>
 </file>
@@ -536,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -566,7 +575,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,7 +917,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -921,7 +929,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -933,7 +941,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -947,7 +955,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -962,67 +970,79 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>9.33</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.96</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>7</v>
+        <v>9.33</v>
       </c>
       <c r="D7" s="7">
-        <v>1</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>114</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1">
+        <v>114</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
         <v>54</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="15">
+      <c r="C11" s="15">
         <v>59.4</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D11" s="8">
         <v>19.600000000000001</v>
       </c>
     </row>
@@ -1036,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,7 +1094,7 @@
     </row>
     <row r="2" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -1102,7 +1122,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1130,7 +1150,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1154,17 +1174,15 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>339</v>
-      </c>
-      <c r="D5" s="7">
-        <v>120</v>
-      </c>
+        <v>760</v>
+      </c>
+      <c r="D5" s="7"/>
       <c r="G5" t="s">
         <v>6</v>
       </c>
@@ -1180,13 +1198,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>760</v>
+        <v>770</v>
       </c>
       <c r="D6" s="7"/>
       <c r="G6" t="s">
@@ -1204,15 +1222,17 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>770</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>37.1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
@@ -1228,16 +1248,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>37.1</v>
+        <v>51.7</v>
       </c>
       <c r="D8" s="7">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -1254,16 +1274,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>51.7</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D9" s="7">
-        <v>5.8</v>
+        <v>0.4</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -1280,16 +1300,18 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>9.8000000000000007</v>
+        <f>AVERAGE(I12:I13)</f>
+        <v>520</v>
       </c>
       <c r="D10" s="7">
-        <v>0.4</v>
+        <f>STDEVA(I12:I13)/SQRT(2)</f>
+        <v>250</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -1306,18 +1328,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1">
-        <f>AVERAGE(I12:I13)</f>
-        <v>520</v>
+        <v>292.5</v>
       </c>
       <c r="D11" s="7">
-        <f>STDEVA(I12:I13)/SQRT(2)</f>
-        <v>250</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="G11" t="s">
         <v>3</v>
@@ -1333,17 +1353,17 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="1">
-        <v>292.5</v>
-      </c>
-      <c r="D12" s="7">
-        <v>163.80000000000001</v>
+      <c r="A12" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="19">
+        <v>115.406329531968</v>
+      </c>
+      <c r="D12" s="20">
+        <v>73.439181551013107</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -1357,16 +1377,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="19">
-        <v>115.406329531968</v>
+        <v>88.8</v>
       </c>
       <c r="D13" s="20">
-        <v>73.439181551013107</v>
+        <v>6.87</v>
       </c>
       <c r="G13" t="s">
         <v>12</v>
@@ -1380,17 +1400,15 @@
     </row>
     <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="22">
-        <v>88.8</v>
-      </c>
-      <c r="D14" s="23">
-        <v>6.87</v>
-      </c>
+        <v>7.5</v>
+      </c>
+      <c r="D14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1400,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,7 +1445,7 @@
     </row>
     <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1439,23 +1457,25 @@
         <v>0.82</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>5.29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D3" s="7"/>
+      <c r="A3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.12479999999999999</v>
+      </c>
       <c r="G3">
         <v>7.43</v>
       </c>
@@ -1468,91 +1488,103 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.2</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>0.32</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.71</v>
-      </c>
+        <v>0.32</v>
+      </c>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
         <f>AVERAGE(G2:G3)</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8" s="7">
         <f>STDEVA(G2:G3)/SQRT(2)</f>
         <v>1.0700000000000032</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>0.24640000000000001</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D9" s="7">
         <v>0.1351</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
         <v>1.6940999814534656</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10" s="7">
         <v>1.8337311851513098</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="15">
+    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="15">
         <v>0.1450937334938032</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D11" s="8">
         <v>5.8905524473255033E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit the method in (Rouet et al., 2005) (`ELISA+Saturation` -> `Radioligand`)
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1826268F-F0B9-4741-A471-1CBBA39F5DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADA13D4-4A18-C54F-A0AA-F26D1D6F2E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
   <si>
     <t>Reference</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>Rouet et al., 2005</t>
-  </si>
-  <si>
-    <t>ELISA plate+Saturation</t>
   </si>
   <si>
     <t>In-house data, 2023</t>
@@ -545,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -573,8 +570,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,7 +887,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,7 +950,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -970,7 +965,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1037,7 +1032,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C11" s="15">
         <v>59.4</v>
@@ -1056,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,7 +1295,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -1331,7 +1326,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
         <v>292.5</v>
@@ -1354,7 +1349,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>9</v>
@@ -1399,13 +1394,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="22">
+      <c r="A14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="15">
         <v>7.5</v>
       </c>
       <c r="D14" s="8"/>
@@ -1420,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1445,7 +1440,7 @@
     </row>
     <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1465,7 +1460,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1532,7 +1527,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -1551,7 +1546,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
         <v>0.24640000000000001</v>
@@ -1562,7 +1557,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -1576,7 +1571,7 @@
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add short-length VEGFR2 binding affinity data from `Cunningham et al., 1999`
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADA13D4-4A18-C54F-A0AA-F26D1D6F2E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4F2910-82FC-994B-B501-223CEB4BF4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="40">
   <si>
     <t>Reference</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Huang et al., 1998 (VEGF-A164)</t>
   </si>
   <si>
-    <t>Cunningham et al., 1999 (monomer)</t>
-  </si>
-  <si>
     <t>Soker et al., 1998</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
     <t>Soker et al., 1996 (HUVEC)</t>
   </si>
   <si>
-    <t>Cunningham et al., 1999 (predimer)</t>
-  </si>
-  <si>
     <t>Rouet et al., 2005</t>
   </si>
   <si>
@@ -274,6 +268,15 @@
   </si>
   <si>
     <t>Whitaker et al., 2001 (Balb/c cell)</t>
+  </si>
+  <si>
+    <t>Cunningham et al., 1999 (full-length predimer)</t>
+  </si>
+  <si>
+    <t>Cunningham et al., 1999 (full-length monomer)</t>
+  </si>
+  <si>
+    <t>Cunningham et al., 1999 (short-length predimer)</t>
   </si>
 </sst>
 </file>
@@ -912,7 +915,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -924,7 +927,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -950,7 +953,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -965,7 +968,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -977,7 +980,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -991,7 +994,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -1005,7 +1008,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -1017,7 +1020,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -1029,7 +1032,7 @@
     </row>
     <row r="11" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>8</v>
@@ -1049,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1148,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1169,7 +1172,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1193,7 +1196,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1217,7 +1220,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -1243,7 +1246,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -1269,16 +1272,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>9.8000000000000007</v>
+        <v>14.5</v>
       </c>
       <c r="D9" s="7">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -1295,45 +1298,45 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>51.7</v>
+      </c>
+      <c r="J10">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
         <f>AVERAGE(I12:I13)</f>
         <v>520</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D11" s="7">
         <f>STDEVA(I12:I13)/SQRT(2)</f>
         <v>250</v>
       </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10">
-        <v>51.7</v>
-      </c>
-      <c r="J10">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1">
-        <v>292.5</v>
-      </c>
-      <c r="D11" s="7">
-        <v>163.80000000000001</v>
-      </c>
       <c r="G11" t="s">
         <v>3</v>
       </c>
@@ -1348,17 +1351,17 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="19">
-        <v>115.406329531968</v>
-      </c>
-      <c r="D12" s="20">
-        <v>73.439181551013107</v>
+      <c r="A12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>292.5</v>
+      </c>
+      <c r="D12" s="7">
+        <v>163.80000000000001</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -1372,16 +1375,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="19">
-        <v>88.8</v>
+        <v>115.406329531968</v>
       </c>
       <c r="D13" s="20">
-        <v>6.87</v>
+        <v>73.439181551013107</v>
       </c>
       <c r="G13" t="s">
         <v>12</v>
@@ -1393,17 +1396,31 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="19">
+        <v>88.8</v>
+      </c>
+      <c r="D14" s="20">
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="15">
         <v>7.5</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1440,7 +1457,7 @@
     </row>
     <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1452,7 +1469,7 @@
         <v>0.82</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2">
         <v>5.29</v>
@@ -1460,7 +1477,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1477,7 +1494,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1489,7 +1506,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1501,7 +1518,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1513,7 +1530,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1527,7 +1544,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -1543,7 +1560,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>8</v>
@@ -1557,7 +1574,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -1571,7 +1588,7 @@
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add VEGFR2 data from `Whitaker et al., 2001`
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4F2910-82FC-994B-B501-223CEB4BF4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7316AB7-35AE-0C44-A2B5-3B936AA99EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="40">
   <si>
     <t>Reference</t>
   </si>
@@ -1052,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1220,16 +1220,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>37.1</v>
+        <v>339</v>
       </c>
       <c r="D7" s="7">
-        <v>4.9000000000000004</v>
+        <v>119.7587</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
@@ -1246,16 +1246,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>51.7</v>
+        <v>291</v>
       </c>
       <c r="D8" s="7">
-        <v>5.8</v>
+        <v>54.363300000000002</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -1272,16 +1272,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>14.5</v>
+        <v>37.1</v>
       </c>
       <c r="D9" s="7">
-        <v>1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -1298,16 +1298,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>9.8000000000000007</v>
+        <v>51.7</v>
       </c>
       <c r="D10" s="7">
-        <v>0.4</v>
+        <v>5.8</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -1324,68 +1324,68 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
         <f>AVERAGE(I12:I13)</f>
         <v>520</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D13" s="7">
         <f>STDEVA(I12:I13)/SQRT(2)</f>
         <v>250</v>
       </c>
-      <c r="G11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="J11">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1">
-        <v>292.5</v>
-      </c>
-      <c r="D12" s="7">
-        <v>163.80000000000001</v>
-      </c>
-      <c r="G12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="19">
-        <v>115.406329531968</v>
-      </c>
-      <c r="D13" s="20">
-        <v>73.439181551013107</v>
-      </c>
       <c r="G13" t="s">
         <v>12</v>
       </c>
@@ -1397,30 +1397,58 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>292.5</v>
+      </c>
+      <c r="D14" s="7">
+        <v>163.80000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="19">
+        <v>115.406329531968</v>
+      </c>
+      <c r="D15" s="20">
+        <v>73.439181551013107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="19">
+      <c r="B16" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="19">
         <v>88.8</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D16" s="20">
         <v>6.87</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="17" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="15">
+      <c r="B17" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="15">
         <v>7.5</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D17" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1432,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add two additional VEGF-A:NRP1 data
</commit_message>
<xml_diff>
--- a/data/binding_affinity.xlsx
+++ b/data/binding_affinity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2599619F-4880-244B-BE08-F43B45886DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A55A60-A8CA-464F-ACAD-E112818E8241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" activeTab="2" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="VEGFA165_VEGFR1" sheetId="3" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="43">
   <si>
     <t>Reference</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Tessler et al., 1994</t>
+  </si>
+  <si>
+    <t>Gluzman-Poltorak et al., 2000</t>
+  </si>
+  <si>
+    <t>Von Wronski et al., 2006</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -576,6 +582,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,7 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1468,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1624,19 +1634,43 @@
         <v>1.8340000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="15">
+      <c r="B11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="19">
         <v>0.14510000000000001</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="20">
         <v>5.8909999999999997E-2</v>
       </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="21">
+        <v>0.18</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="D13" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>